<commit_message>
Add support for amq song export that plays failed songs from a game
</commit_message>
<xml_diff>
--- a/AMQDB.xlsx
+++ b/AMQDB.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15960" uniqueCount="2007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15950" uniqueCount="2007">
   <si>
     <t>ID</t>
   </si>
@@ -50902,13 +50902,13 @@
     <row r="211">
       <c r="A211" s="3"/>
       <c r="B211" s="4" t="s">
-        <v>568</v>
+        <v>605</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D211" s="5" t="s">
-        <v>569</v>
+        <v>606</v>
       </c>
       <c r="E211" s="5" t="s">
         <v>10</v>
@@ -50921,13 +50921,13 @@
     <row r="212">
       <c r="A212" s="3"/>
       <c r="B212" s="4" t="s">
-        <v>568</v>
+        <v>607</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D212" s="5" t="s">
-        <v>570</v>
+        <v>608</v>
       </c>
       <c r="E212" s="5" t="s">
         <v>10</v>
@@ -50940,13 +50940,13 @@
     <row r="213">
       <c r="A213" s="3"/>
       <c r="B213" s="4" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D213" s="5" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="E213" s="5" t="s">
         <v>10</v>
@@ -50959,13 +50959,13 @@
     <row r="214">
       <c r="A214" s="3"/>
       <c r="B214" s="4" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D214" s="5" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="E214" s="5" t="s">
         <v>10</v>
@@ -50978,13 +50978,13 @@
     <row r="215">
       <c r="A215" s="3"/>
       <c r="B215" s="4" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D215" s="5" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="E215" s="5" t="s">
         <v>10</v>
@@ -50997,13 +50997,13 @@
     <row r="216">
       <c r="A216" s="3"/>
       <c r="B216" s="4" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D216" s="5" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="E216" s="5" t="s">
         <v>10</v>
@@ -51016,13 +51016,13 @@
     <row r="217">
       <c r="A217" s="3"/>
       <c r="B217" s="4" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="D217" s="5" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
       <c r="E217" s="5" t="s">
         <v>10</v>
@@ -51035,13 +51035,13 @@
     <row r="218">
       <c r="A218" s="3"/>
       <c r="B218" s="4" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D218" s="5" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="E218" s="5" t="s">
         <v>10</v>
@@ -51054,13 +51054,13 @@
     <row r="219">
       <c r="A219" s="3"/>
       <c r="B219" s="4" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D219" s="5" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="E219" s="5" t="s">
         <v>10</v>
@@ -51073,13 +51073,13 @@
     <row r="220">
       <c r="A220" s="3"/>
       <c r="B220" s="4" t="s">
-        <v>619</v>
+        <v>630</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D220" s="5" t="s">
-        <v>620</v>
+        <v>631</v>
       </c>
       <c r="E220" s="5" t="s">
         <v>10</v>
@@ -51092,13 +51092,13 @@
     <row r="221">
       <c r="A221" s="3"/>
       <c r="B221" s="4" t="s">
-        <v>621</v>
+        <v>632</v>
       </c>
       <c r="C221" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D221" s="5" t="s">
-        <v>622</v>
+        <v>633</v>
       </c>
       <c r="E221" s="5" t="s">
         <v>10</v>
@@ -51111,13 +51111,13 @@
     <row r="222">
       <c r="A222" s="3"/>
       <c r="B222" s="4" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="C222" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D222" s="5" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="E222" s="5" t="s">
         <v>10</v>
@@ -51130,13 +51130,13 @@
     <row r="223">
       <c r="A223" s="3"/>
       <c r="B223" s="4" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D223" s="5" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="E223" s="5" t="s">
         <v>10</v>
@@ -51149,13 +51149,13 @@
     <row r="224">
       <c r="A224" s="3"/>
       <c r="B224" s="4" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="5" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="E224" s="5" t="s">
         <v>10</v>
@@ -51168,13 +51168,13 @@
     <row r="225">
       <c r="A225" s="3"/>
       <c r="B225" s="4" t="s">
-        <v>636</v>
+        <v>647</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D225" s="5" t="s">
-        <v>637</v>
+        <v>648</v>
       </c>
       <c r="E225" s="5" t="s">
         <v>10</v>
@@ -51187,13 +51187,13 @@
     <row r="226">
       <c r="A226" s="3"/>
       <c r="B226" s="4" t="s">
-        <v>640</v>
+        <v>651</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D226" s="5" t="s">
-        <v>641</v>
+        <v>652</v>
       </c>
       <c r="E226" s="5" t="s">
         <v>10</v>
@@ -51206,13 +51206,13 @@
     <row r="227">
       <c r="A227" s="3"/>
       <c r="B227" s="4" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D227" s="5" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="E227" s="5" t="s">
         <v>10</v>
@@ -51225,13 +51225,13 @@
     <row r="228">
       <c r="A228" s="3"/>
       <c r="B228" s="4" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D228" s="5" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="E228" s="5" t="s">
         <v>10</v>
@@ -51244,13 +51244,13 @@
     <row r="229">
       <c r="A229" s="3"/>
       <c r="B229" s="4" t="s">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D229" s="5" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="E229" s="5" t="s">
         <v>10</v>
@@ -51263,13 +51263,13 @@
     <row r="230">
       <c r="A230" s="3"/>
       <c r="B230" s="4" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D230" s="5" t="s">
-        <v>655</v>
+        <v>662</v>
       </c>
       <c r="E230" s="5" t="s">
         <v>10</v>
@@ -51282,13 +51282,13 @@
     <row r="231">
       <c r="A231" s="3"/>
       <c r="B231" s="4" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D231" s="5" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="E231" s="5" t="s">
         <v>10</v>
@@ -51304,10 +51304,10 @@
         <v>661</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D232" s="5" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="E232" s="5" t="s">
         <v>10</v>
@@ -51323,10 +51323,10 @@
         <v>661</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="D233" s="5" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="E233" s="5" t="s">
         <v>10</v>
@@ -51342,10 +51342,10 @@
         <v>661</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D234" s="5" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="E234" s="5" t="s">
         <v>10</v>
@@ -51361,10 +51361,10 @@
         <v>661</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D235" s="5" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="E235" s="5" t="s">
         <v>10</v>
@@ -51380,10 +51380,10 @@
         <v>661</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D236" s="5" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="E236" s="5" t="s">
         <v>10</v>
@@ -51396,13 +51396,13 @@
     <row r="237">
       <c r="A237" s="3"/>
       <c r="B237" s="4" t="s">
-        <v>661</v>
+        <v>669</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D237" s="5" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="E237" s="5" t="s">
         <v>10</v>
@@ -51415,13 +51415,13 @@
     <row r="238">
       <c r="A238" s="3"/>
       <c r="B238" s="4" t="s">
-        <v>661</v>
+        <v>675</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D238" s="5" t="s">
-        <v>668</v>
+        <v>676</v>
       </c>
       <c r="E238" s="5" t="s">
         <v>10</v>
@@ -51434,13 +51434,13 @@
     <row r="239">
       <c r="A239" s="3"/>
       <c r="B239" s="4" t="s">
-        <v>669</v>
+        <v>677</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D239" s="5" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="E239" s="5" t="s">
         <v>10</v>
@@ -51453,13 +51453,13 @@
     <row r="240">
       <c r="A240" s="3"/>
       <c r="B240" s="4" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D240" s="5" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="E240" s="5" t="s">
         <v>10</v>
@@ -51472,15 +51472,15 @@
     <row r="241">
       <c r="A241" s="3"/>
       <c r="B241" s="4" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="C241" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D241" s="5" t="s">
-        <v>678</v>
-      </c>
-      <c r="E241" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="E241" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F241" s="6" t="s">
@@ -51491,13 +51491,13 @@
     <row r="242">
       <c r="A242" s="3"/>
       <c r="B242" s="4" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D242" s="5" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="E242" s="5" t="s">
         <v>10</v>
@@ -51510,15 +51510,15 @@
     <row r="243">
       <c r="A243" s="3"/>
       <c r="B243" s="4" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D243" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="E243" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="E243" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F243" s="6" t="s">
@@ -51529,18 +51529,18 @@
     <row r="244">
       <c r="A244" s="3"/>
       <c r="B244" s="4" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D244" s="5" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="E244" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F244" s="6" t="s">
+      <c r="F244" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G244" s="3"/>
@@ -51548,13 +51548,13 @@
     <row r="245">
       <c r="A245" s="3"/>
       <c r="B245" s="4" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D245" s="5" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="E245" s="5" t="s">
         <v>10</v>
@@ -51567,13 +51567,13 @@
     <row r="246">
       <c r="A246" s="3"/>
       <c r="B246" s="4" t="s">
-        <v>687</v>
+        <v>692</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D246" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="E246" s="5" t="s">
         <v>10</v>
@@ -51586,13 +51586,13 @@
     <row r="247">
       <c r="A247" s="3"/>
       <c r="B247" s="4" t="s">
-        <v>689</v>
+        <v>694</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D247" s="5" t="s">
-        <v>690</v>
+        <v>695</v>
       </c>
       <c r="E247" s="5" t="s">
         <v>10</v>
@@ -51605,18 +51605,18 @@
     <row r="248">
       <c r="A248" s="3"/>
       <c r="B248" s="4" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D248" s="5" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="E248" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F248" s="4" t="s">
+      <c r="F248" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G248" s="3"/>
@@ -51624,13 +51624,13 @@
     <row r="249">
       <c r="A249" s="3"/>
       <c r="B249" s="4" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D249" s="5" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="E249" s="5" t="s">
         <v>10</v>
@@ -51643,13 +51643,13 @@
     <row r="250">
       <c r="A250" s="3"/>
       <c r="B250" s="4" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="E250" s="5" t="s">
         <v>10</v>
@@ -51662,13 +51662,13 @@
     <row r="251">
       <c r="A251" s="3"/>
       <c r="B251" s="4" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D251" s="5" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="E251" s="5" t="s">
         <v>10</v>
@@ -51681,13 +51681,13 @@
     <row r="252">
       <c r="A252" s="3"/>
       <c r="B252" s="4" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="C252" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D252" s="5" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="E252" s="5" t="s">
         <v>10</v>
@@ -51700,13 +51700,13 @@
     <row r="253">
       <c r="A253" s="3"/>
       <c r="B253" s="4" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D253" s="5" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="E253" s="5" t="s">
         <v>10</v>
@@ -51722,10 +51722,10 @@
         <v>703</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D254" s="5" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="E254" s="5" t="s">
         <v>10</v>
@@ -51738,13 +51738,13 @@
     <row r="255">
       <c r="A255" s="3"/>
       <c r="B255" s="4" t="s">
-        <v>703</v>
+        <v>715</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>705</v>
+        <v>716</v>
       </c>
       <c r="E255" s="5" t="s">
         <v>10</v>
@@ -51757,13 +51757,13 @@
     <row r="256">
       <c r="A256" s="3"/>
       <c r="B256" s="4" t="s">
-        <v>703</v>
+        <v>715</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D256" s="5" t="s">
-        <v>706</v>
+        <v>717</v>
       </c>
       <c r="E256" s="5" t="s">
         <v>10</v>
@@ -51776,13 +51776,13 @@
     <row r="257">
       <c r="A257" s="3"/>
       <c r="B257" s="4" t="s">
-        <v>715</v>
+        <v>720</v>
       </c>
       <c r="C257" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D257" s="5" t="s">
-        <v>716</v>
+        <v>721</v>
       </c>
       <c r="E257" s="5" t="s">
         <v>10</v>
@@ -51795,13 +51795,13 @@
     <row r="258">
       <c r="A258" s="3"/>
       <c r="B258" s="4" t="s">
-        <v>715</v>
+        <v>722</v>
       </c>
       <c r="C258" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D258" s="5" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="E258" s="5" t="s">
         <v>10</v>
@@ -51814,13 +51814,13 @@
     <row r="259">
       <c r="A259" s="3"/>
       <c r="B259" s="4" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="C259" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D259" s="5" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="E259" s="5" t="s">
         <v>10</v>
@@ -51833,13 +51833,13 @@
     <row r="260">
       <c r="A260" s="3"/>
       <c r="B260" s="4" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D260" s="5" t="s">
-        <v>723</v>
+        <v>731</v>
       </c>
       <c r="E260" s="5" t="s">
         <v>10</v>
@@ -51852,13 +51852,13 @@
     <row r="261">
       <c r="A261" s="3"/>
       <c r="B261" s="4" t="s">
-        <v>724</v>
+        <v>732</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
       <c r="E261" s="5" t="s">
         <v>10</v>
@@ -51871,13 +51871,13 @@
     <row r="262">
       <c r="A262" s="3"/>
       <c r="B262" s="4" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D262" s="5" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c r="E262" s="5" t="s">
         <v>10</v>
@@ -51890,13 +51890,13 @@
     <row r="263">
       <c r="A263" s="3"/>
       <c r="B263" s="4" t="s">
-        <v>732</v>
+        <v>738</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D263" s="5" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="E263" s="5" t="s">
         <v>10</v>
@@ -51909,13 +51909,13 @@
     <row r="264">
       <c r="A264" s="3"/>
       <c r="B264" s="4" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
       <c r="C264" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D264" s="5" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c r="E264" s="5" t="s">
         <v>10</v>
@@ -51928,13 +51928,13 @@
     <row r="265">
       <c r="A265" s="3"/>
       <c r="B265" s="4" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D265" s="5" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="E265" s="5" t="s">
         <v>10</v>
@@ -51947,13 +51947,13 @@
     <row r="266">
       <c r="A266" s="3"/>
       <c r="B266" s="4" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D266" s="5" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="E266" s="5" t="s">
         <v>10</v>
@@ -51966,13 +51966,13 @@
     <row r="267">
       <c r="A267" s="3"/>
       <c r="B267" s="4" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D267" s="5" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="E267" s="5" t="s">
         <v>10</v>
@@ -51985,13 +51985,13 @@
     <row r="268">
       <c r="A268" s="3"/>
       <c r="B268" s="4" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D268" s="5" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="E268" s="5" t="s">
         <v>10</v>
@@ -52004,13 +52004,13 @@
     <row r="269">
       <c r="A269" s="3"/>
       <c r="B269" s="4" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="C269" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D269" s="5" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="E269" s="5" t="s">
         <v>10</v>
@@ -52023,13 +52023,13 @@
     <row r="270">
       <c r="A270" s="3"/>
       <c r="B270" s="4" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D270" s="5" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="E270" s="5" t="s">
         <v>10</v>
@@ -52042,13 +52042,13 @@
     <row r="271">
       <c r="A271" s="3"/>
       <c r="B271" s="4" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D271" s="5" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="E271" s="5" t="s">
         <v>10</v>
@@ -52061,13 +52061,13 @@
     <row r="272">
       <c r="A272" s="3"/>
       <c r="B272" s="4" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D272" s="5" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="E272" s="5" t="s">
         <v>10</v>
@@ -52080,13 +52080,13 @@
     <row r="273">
       <c r="A273" s="3"/>
       <c r="B273" s="4" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D273" s="5" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="E273" s="5" t="s">
         <v>10</v>
@@ -52099,13 +52099,13 @@
     <row r="274">
       <c r="A274" s="3"/>
       <c r="B274" s="4" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="C274" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D274" s="5" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="E274" s="5" t="s">
         <v>10</v>
@@ -52118,13 +52118,13 @@
     <row r="275">
       <c r="A275" s="3"/>
       <c r="B275" s="4" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="C275" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D275" s="5" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="E275" s="5" t="s">
         <v>10</v>
@@ -52137,13 +52137,13 @@
     <row r="276">
       <c r="A276" s="3"/>
       <c r="B276" s="4" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D276" s="5" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c r="E276" s="5" t="s">
         <v>10</v>
@@ -52156,13 +52156,13 @@
     <row r="277">
       <c r="A277" s="3"/>
       <c r="B277" s="4" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D277" s="5" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="E277" s="5" t="s">
         <v>10</v>
@@ -52178,10 +52178,10 @@
         <v>762</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D278" s="5" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="E278" s="5" t="s">
         <v>10</v>
@@ -52194,13 +52194,13 @@
     <row r="279">
       <c r="A279" s="3"/>
       <c r="B279" s="4" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D279" s="5" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="E279" s="5" t="s">
         <v>10</v>
@@ -52213,13 +52213,13 @@
     <row r="280">
       <c r="A280" s="3"/>
       <c r="B280" s="4" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="D280" s="5" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="E280" s="5" t="s">
         <v>10</v>
@@ -52232,13 +52232,13 @@
     <row r="281">
       <c r="A281" s="3"/>
       <c r="B281" s="4" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="C281" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D281" s="5" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="E281" s="5" t="s">
         <v>10</v>
@@ -52251,13 +52251,13 @@
     <row r="282">
       <c r="A282" s="3"/>
       <c r="B282" s="4" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D282" s="5" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="E282" s="5" t="s">
         <v>10</v>
@@ -52270,13 +52270,13 @@
     <row r="283">
       <c r="A283" s="3"/>
       <c r="B283" s="4" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="C283" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D283" s="5" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
       <c r="E283" s="5" t="s">
         <v>10</v>
@@ -52289,13 +52289,13 @@
     <row r="284">
       <c r="A284" s="3"/>
       <c r="B284" s="4" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="C284" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D284" s="5" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="E284" s="5" t="s">
         <v>10</v>
@@ -52308,13 +52308,13 @@
     <row r="285">
       <c r="A285" s="3"/>
       <c r="B285" s="4" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D285" s="5" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="E285" s="5" t="s">
         <v>10</v>
@@ -52327,13 +52327,13 @@
     <row r="286">
       <c r="A286" s="3"/>
       <c r="B286" s="4" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C286" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D286" s="5" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="E286" s="5" t="s">
         <v>10</v>
@@ -52346,13 +52346,13 @@
     <row r="287">
       <c r="A287" s="3"/>
       <c r="B287" s="4" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="C287" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D287" s="5" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
       <c r="E287" s="5" t="s">
         <v>10</v>
@@ -52368,10 +52368,10 @@
         <v>781</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D288" s="5" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="E288" s="5" t="s">
         <v>10</v>
@@ -52387,10 +52387,10 @@
         <v>781</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="D289" s="5" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="E289" s="5" t="s">
         <v>10</v>
@@ -52406,10 +52406,10 @@
         <v>781</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D290" s="5" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="E290" s="5" t="s">
         <v>10</v>
@@ -52425,10 +52425,10 @@
         <v>781</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="D291" s="5" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="E291" s="5" t="s">
         <v>10</v>
@@ -52441,13 +52441,13 @@
     <row r="292">
       <c r="A292" s="3"/>
       <c r="B292" s="4" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D292" s="5" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c r="E292" s="5" t="s">
         <v>10</v>
@@ -52460,13 +52460,13 @@
     <row r="293">
       <c r="A293" s="3"/>
       <c r="B293" s="4" t="s">
-        <v>781</v>
+        <v>806</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="D293" s="5" t="s">
-        <v>787</v>
+        <v>807</v>
       </c>
       <c r="E293" s="5" t="s">
         <v>10</v>
@@ -52479,13 +52479,13 @@
     <row r="294">
       <c r="A294" s="3"/>
       <c r="B294" s="4" t="s">
-        <v>791</v>
+        <v>810</v>
       </c>
       <c r="C294" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D294" s="5" t="s">
-        <v>792</v>
+        <v>811</v>
       </c>
       <c r="E294" s="5" t="s">
         <v>10</v>
@@ -52498,13 +52498,13 @@
     <row r="295">
       <c r="A295" s="3"/>
       <c r="B295" s="4" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="C295" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D295" s="5" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
       <c r="E295" s="5" t="s">
         <v>10</v>
@@ -52517,13 +52517,13 @@
     <row r="296">
       <c r="A296" s="3"/>
       <c r="B296" s="4" t="s">
-        <v>810</v>
+        <v>816</v>
       </c>
       <c r="C296" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D296" s="5" t="s">
-        <v>811</v>
+        <v>817</v>
       </c>
       <c r="E296" s="5" t="s">
         <v>10</v>
@@ -52536,13 +52536,13 @@
     <row r="297">
       <c r="A297" s="3"/>
       <c r="B297" s="4" t="s">
-        <v>810</v>
+        <v>818</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D297" s="5" t="s">
-        <v>812</v>
+        <v>819</v>
       </c>
       <c r="E297" s="5" t="s">
         <v>10</v>
@@ -52555,13 +52555,13 @@
     <row r="298">
       <c r="A298" s="3"/>
       <c r="B298" s="4" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D298" s="5" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="E298" s="5" t="s">
         <v>10</v>
@@ -52574,13 +52574,13 @@
     <row r="299">
       <c r="A299" s="3"/>
       <c r="B299" s="4" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="C299" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D299" s="5" t="s">
-        <v>819</v>
+        <v>837</v>
       </c>
       <c r="E299" s="5" t="s">
         <v>10</v>
@@ -52593,13 +52593,13 @@
     <row r="300">
       <c r="A300" s="3"/>
       <c r="B300" s="4" t="s">
-        <v>818</v>
+        <v>846</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D300" s="5" t="s">
-        <v>820</v>
+        <v>847</v>
       </c>
       <c r="E300" s="5" t="s">
         <v>10</v>
@@ -52612,13 +52612,13 @@
     <row r="301">
       <c r="A301" s="3"/>
       <c r="B301" s="4" t="s">
-        <v>836</v>
+        <v>848</v>
       </c>
       <c r="C301" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D301" s="5" t="s">
-        <v>837</v>
+        <v>849</v>
       </c>
       <c r="E301" s="5" t="s">
         <v>10</v>
@@ -52631,13 +52631,13 @@
     <row r="302">
       <c r="A302" s="3"/>
       <c r="B302" s="4" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="C302" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D302" s="5" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="E302" s="5" t="s">
         <v>10</v>
@@ -52650,13 +52650,13 @@
     <row r="303">
       <c r="A303" s="3"/>
       <c r="B303" s="4" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="C303" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D303" s="5" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="E303" s="5" t="s">
         <v>10</v>
@@ -52669,13 +52669,13 @@
     <row r="304">
       <c r="A304" s="3"/>
       <c r="B304" s="4" t="s">
-        <v>850</v>
+        <v>861</v>
       </c>
       <c r="C304" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D304" s="5" t="s">
-        <v>851</v>
+        <v>862</v>
       </c>
       <c r="E304" s="5" t="s">
         <v>10</v>
@@ -52688,13 +52688,13 @@
     <row r="305">
       <c r="A305" s="3"/>
       <c r="B305" s="4" t="s">
-        <v>852</v>
+        <v>863</v>
       </c>
       <c r="C305" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D305" s="5" t="s">
-        <v>853</v>
+        <v>864</v>
       </c>
       <c r="E305" s="5" t="s">
         <v>10</v>
@@ -52707,13 +52707,13 @@
     <row r="306">
       <c r="A306" s="3"/>
       <c r="B306" s="4" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C306" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D306" s="5" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="E306" s="5" t="s">
         <v>10</v>
@@ -52726,13 +52726,13 @@
     <row r="307">
       <c r="A307" s="3"/>
       <c r="B307" s="4" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D307" s="5" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="E307" s="5" t="s">
         <v>10</v>
@@ -52745,13 +52745,13 @@
     <row r="308">
       <c r="A308" s="3"/>
       <c r="B308" s="4" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="C308" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D308" s="5" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="E308" s="5" t="s">
         <v>10</v>
@@ -52764,13 +52764,13 @@
     <row r="309">
       <c r="A309" s="3"/>
       <c r="B309" s="4" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="C309" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D309" s="5" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
       <c r="E309" s="5" t="s">
         <v>10</v>
@@ -52783,13 +52783,13 @@
     <row r="310">
       <c r="A310" s="3"/>
       <c r="B310" s="4" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="C310" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="E310" s="5" t="s">
         <v>10</v>
@@ -52802,13 +52802,13 @@
     <row r="311">
       <c r="A311" s="3"/>
       <c r="B311" s="4" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="C311" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
       <c r="E311" s="5" t="s">
         <v>10</v>
@@ -52821,13 +52821,13 @@
     <row r="312">
       <c r="A312" s="3"/>
       <c r="B312" s="4" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="E312" s="5" t="s">
         <v>10</v>
@@ -52840,13 +52840,13 @@
     <row r="313">
       <c r="A313" s="3"/>
       <c r="B313" s="4" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="C313" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="E313" s="5" t="s">
         <v>10</v>
@@ -52859,13 +52859,13 @@
     <row r="314">
       <c r="A314" s="3"/>
       <c r="B314" s="4" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="C314" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="E314" s="5" t="s">
         <v>10</v>
@@ -52878,13 +52878,13 @@
     <row r="315">
       <c r="A315" s="3"/>
       <c r="B315" s="4" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="C315" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D315" s="5" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c r="E315" s="5" t="s">
         <v>10</v>
@@ -52897,13 +52897,13 @@
     <row r="316">
       <c r="A316" s="3"/>
       <c r="B316" s="4" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="E316" s="5" t="s">
         <v>10</v>
@@ -52916,13 +52916,13 @@
     <row r="317">
       <c r="A317" s="3"/>
       <c r="B317" s="4" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="E317" s="5" t="s">
         <v>10</v>
@@ -52935,13 +52935,13 @@
     <row r="318">
       <c r="A318" s="3"/>
       <c r="B318" s="4" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="C318" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="E318" s="5" t="s">
         <v>10</v>
@@ -52954,13 +52954,13 @@
     <row r="319">
       <c r="A319" s="3"/>
       <c r="B319" s="4" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="C319" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D319" s="5" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="E319" s="5" t="s">
         <v>10</v>
@@ -52973,13 +52973,13 @@
     <row r="320">
       <c r="A320" s="3"/>
       <c r="B320" s="4" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="C320" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D320" s="5" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="E320" s="5" t="s">
         <v>10</v>
@@ -52992,13 +52992,13 @@
     <row r="321">
       <c r="A321" s="3"/>
       <c r="B321" s="4" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="C321" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D321" s="5" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="E321" s="5" t="s">
         <v>10</v>
@@ -53011,13 +53011,13 @@
     <row r="322">
       <c r="A322" s="3"/>
       <c r="B322" s="4" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="C322" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D322" s="5" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="E322" s="5" t="s">
         <v>10</v>
@@ -53030,13 +53030,13 @@
     <row r="323">
       <c r="A323" s="3"/>
       <c r="B323" s="4" t="s">
-        <v>891</v>
+        <v>896</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D323" s="5" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
       <c r="E323" s="5" t="s">
         <v>10</v>
@@ -53049,13 +53049,13 @@
     <row r="324">
       <c r="A324" s="3"/>
       <c r="B324" s="4" t="s">
-        <v>894</v>
+        <v>909</v>
       </c>
       <c r="C324" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D324" s="5" t="s">
-        <v>895</v>
+        <v>910</v>
       </c>
       <c r="E324" s="5" t="s">
         <v>10</v>
@@ -53068,13 +53068,13 @@
     <row r="325">
       <c r="A325" s="3"/>
       <c r="B325" s="4" t="s">
-        <v>896</v>
+        <v>916</v>
       </c>
       <c r="C325" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D325" s="5" t="s">
-        <v>897</v>
+        <v>917</v>
       </c>
       <c r="E325" s="5" t="s">
         <v>10</v>
@@ -53087,13 +53087,13 @@
     <row r="326">
       <c r="A326" s="3"/>
       <c r="B326" s="4" t="s">
-        <v>909</v>
+        <v>916</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D326" s="5" t="s">
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="E326" s="5" t="s">
         <v>10</v>
@@ -53106,13 +53106,13 @@
     <row r="327">
       <c r="A327" s="3"/>
       <c r="B327" s="4" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="C327" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D327" s="5" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="E327" s="5" t="s">
         <v>10</v>
@@ -53125,13 +53125,13 @@
     <row r="328">
       <c r="A328" s="3"/>
       <c r="B328" s="4" t="s">
-        <v>916</v>
+        <v>923</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D328" s="5" t="s">
-        <v>918</v>
+        <v>924</v>
       </c>
       <c r="E328" s="5" t="s">
         <v>10</v>
@@ -53144,13 +53144,13 @@
     <row r="329">
       <c r="A329" s="3"/>
       <c r="B329" s="4" t="s">
-        <v>919</v>
+        <v>925</v>
       </c>
       <c r="C329" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D329" s="5" t="s">
-        <v>920</v>
+        <v>926</v>
       </c>
       <c r="E329" s="5" t="s">
         <v>10</v>
@@ -53163,13 +53163,13 @@
     <row r="330">
       <c r="A330" s="3"/>
       <c r="B330" s="4" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="C330" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D330" s="5" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c r="E330" s="5" t="s">
         <v>10</v>
@@ -53182,13 +53182,13 @@
     <row r="331">
       <c r="A331" s="3"/>
       <c r="B331" s="4" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C331" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D331" s="5" t="s">
-        <v>926</v>
+        <v>934</v>
       </c>
       <c r="E331" s="5" t="s">
         <v>10</v>
@@ -53201,13 +53201,13 @@
     <row r="332">
       <c r="A332" s="3"/>
       <c r="B332" s="4" t="s">
-        <v>927</v>
+        <v>935</v>
       </c>
       <c r="C332" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D332" s="5" t="s">
-        <v>928</v>
+        <v>936</v>
       </c>
       <c r="E332" s="5" t="s">
         <v>10</v>
@@ -53220,13 +53220,13 @@
     <row r="333">
       <c r="A333" s="3"/>
       <c r="B333" s="4" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C333" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D333" s="5" t="s">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c r="E333" s="5" t="s">
         <v>10</v>
@@ -53239,13 +53239,13 @@
     <row r="334">
       <c r="A334" s="3"/>
       <c r="B334" s="4" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c r="C334" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D334" s="5" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="E334" s="5" t="s">
         <v>10</v>
@@ -53258,13 +53258,13 @@
     <row r="335">
       <c r="A335" s="3"/>
       <c r="B335" s="4" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c r="C335" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D335" s="5" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="E335" s="5" t="s">
         <v>10</v>
@@ -53277,13 +53277,13 @@
     <row r="336">
       <c r="A336" s="3"/>
       <c r="B336" s="4" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="C336" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D336" s="5" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="E336" s="5" t="s">
         <v>10</v>
@@ -53296,13 +53296,13 @@
     <row r="337">
       <c r="A337" s="3"/>
       <c r="B337" s="4" t="s">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c r="C337" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D337" s="5" t="s">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="E337" s="5" t="s">
         <v>10</v>
@@ -53315,13 +53315,13 @@
     <row r="338">
       <c r="A338" s="3"/>
       <c r="B338" s="4" t="s">
-        <v>943</v>
+        <v>949</v>
       </c>
       <c r="C338" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D338" s="5" t="s">
-        <v>944</v>
+        <v>950</v>
       </c>
       <c r="E338" s="5" t="s">
         <v>10</v>
@@ -53334,13 +53334,13 @@
     <row r="339">
       <c r="A339" s="3"/>
       <c r="B339" s="4" t="s">
-        <v>945</v>
+        <v>951</v>
       </c>
       <c r="C339" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D339" s="5" t="s">
-        <v>946</v>
+        <v>952</v>
       </c>
       <c r="E339" s="5" t="s">
         <v>10</v>
@@ -53353,13 +53353,13 @@
     <row r="340">
       <c r="A340" s="3"/>
       <c r="B340" s="4" t="s">
-        <v>949</v>
+        <v>955</v>
       </c>
       <c r="C340" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D340" s="5" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="E340" s="5" t="s">
         <v>10</v>
@@ -53372,13 +53372,13 @@
     <row r="341">
       <c r="A341" s="3"/>
       <c r="B341" s="4" t="s">
-        <v>951</v>
+        <v>957</v>
       </c>
       <c r="C341" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D341" s="5" t="s">
-        <v>952</v>
+        <v>958</v>
       </c>
       <c r="E341" s="5" t="s">
         <v>10</v>
@@ -53391,13 +53391,13 @@
     <row r="342">
       <c r="A342" s="3"/>
       <c r="B342" s="4" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="C342" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D342" s="5" t="s">
-        <v>956</v>
+        <v>960</v>
       </c>
       <c r="E342" s="5" t="s">
         <v>10</v>
@@ -53410,13 +53410,13 @@
     <row r="343">
       <c r="A343" s="3"/>
       <c r="B343" s="4" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="C343" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D343" s="5" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="E343" s="5" t="s">
         <v>10</v>
@@ -53429,13 +53429,13 @@
     <row r="344">
       <c r="A344" s="3"/>
       <c r="B344" s="4" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="C344" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D344" s="5" t="s">
-        <v>960</v>
+        <v>964</v>
       </c>
       <c r="E344" s="5" t="s">
         <v>10</v>
@@ -53448,13 +53448,13 @@
     <row r="345">
       <c r="A345" s="3"/>
       <c r="B345" s="4" t="s">
-        <v>961</v>
+        <v>965</v>
       </c>
       <c r="C345" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D345" s="5" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="E345" s="5" t="s">
         <v>10</v>
@@ -53467,13 +53467,13 @@
     <row r="346">
       <c r="A346" s="3"/>
       <c r="B346" s="4" t="s">
-        <v>963</v>
+        <v>969</v>
       </c>
       <c r="C346" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D346" s="5" t="s">
-        <v>964</v>
+        <v>970</v>
       </c>
       <c r="E346" s="5" t="s">
         <v>10</v>
@@ -53486,13 +53486,13 @@
     <row r="347">
       <c r="A347" s="3"/>
       <c r="B347" s="4" t="s">
-        <v>965</v>
+        <v>971</v>
       </c>
       <c r="C347" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D347" s="5" t="s">
-        <v>966</v>
+        <v>972</v>
       </c>
       <c r="E347" s="5" t="s">
         <v>10</v>
@@ -53505,13 +53505,13 @@
     <row r="348">
       <c r="A348" s="3"/>
       <c r="B348" s="4" t="s">
-        <v>969</v>
+        <v>973</v>
       </c>
       <c r="C348" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D348" s="5" t="s">
-        <v>970</v>
+        <v>974</v>
       </c>
       <c r="E348" s="5" t="s">
         <v>10</v>
@@ -53524,13 +53524,13 @@
     <row r="349">
       <c r="A349" s="3"/>
       <c r="B349" s="4" t="s">
-        <v>971</v>
+        <v>975</v>
       </c>
       <c r="C349" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D349" s="5" t="s">
-        <v>972</v>
+        <v>976</v>
       </c>
       <c r="E349" s="5" t="s">
         <v>10</v>
@@ -53543,13 +53543,13 @@
     <row r="350">
       <c r="A350" s="3"/>
       <c r="B350" s="4" t="s">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c r="C350" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D350" s="5" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="E350" s="5" t="s">
         <v>10</v>
@@ -53562,13 +53562,13 @@
     <row r="351">
       <c r="A351" s="3"/>
       <c r="B351" s="4" t="s">
-        <v>975</v>
+        <v>981</v>
       </c>
       <c r="C351" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D351" s="5" t="s">
-        <v>976</v>
+        <v>982</v>
       </c>
       <c r="E351" s="5" t="s">
         <v>10</v>
@@ -53581,13 +53581,13 @@
     <row r="352">
       <c r="A352" s="3"/>
       <c r="B352" s="4" t="s">
-        <v>977</v>
+        <v>983</v>
       </c>
       <c r="C352" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D352" s="5" t="s">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="E352" s="5" t="s">
         <v>10</v>
@@ -53600,13 +53600,13 @@
     <row r="353">
       <c r="A353" s="3"/>
       <c r="B353" s="4" t="s">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="C353" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D353" s="5" t="s">
-        <v>982</v>
+        <v>988</v>
       </c>
       <c r="E353" s="5" t="s">
         <v>10</v>
@@ -53619,13 +53619,13 @@
     <row r="354">
       <c r="A354" s="3"/>
       <c r="B354" s="4" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="C354" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D354" s="5" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="E354" s="5" t="s">
         <v>10</v>
@@ -53638,13 +53638,13 @@
     <row r="355">
       <c r="A355" s="3"/>
       <c r="B355" s="4" t="s">
-        <v>987</v>
+        <v>991</v>
       </c>
       <c r="C355" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D355" s="5" t="s">
-        <v>988</v>
+        <v>992</v>
       </c>
       <c r="E355" s="5" t="s">
         <v>10</v>
@@ -53657,13 +53657,13 @@
     <row r="356">
       <c r="A356" s="3"/>
       <c r="B356" s="4" t="s">
-        <v>989</v>
+        <v>993</v>
       </c>
       <c r="C356" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D356" s="5" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="E356" s="5" t="s">
         <v>10</v>
@@ -53676,13 +53676,13 @@
     <row r="357">
       <c r="A357" s="3"/>
       <c r="B357" s="4" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="C357" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D357" s="5" t="s">
-        <v>992</v>
+        <v>996</v>
       </c>
       <c r="E357" s="5" t="s">
         <v>10</v>
@@ -53695,13 +53695,13 @@
     <row r="358">
       <c r="A358" s="3"/>
       <c r="B358" s="4" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D358" s="5" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
       <c r="E358" s="5" t="s">
         <v>10</v>
@@ -53714,13 +53714,13 @@
     <row r="359">
       <c r="A359" s="3"/>
       <c r="B359" s="4" t="s">
-        <v>995</v>
+        <v>998</v>
       </c>
       <c r="C359" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D359" s="5" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
       <c r="E359" s="5" t="s">
         <v>10</v>
@@ -53733,15 +53733,15 @@
     <row r="360">
       <c r="A360" s="3"/>
       <c r="B360" s="4" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D360" s="5" t="s">
-        <v>997</v>
-      </c>
-      <c r="E360" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E360" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F360" s="6" t="s">
@@ -53752,59 +53752,21 @@
     <row r="361">
       <c r="A361" s="3"/>
       <c r="B361" s="4" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="C361" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D361" s="5" t="s">
-        <v>999</v>
-      </c>
-      <c r="E361" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E361" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F361" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G361" s="3"/>
-    </row>
-    <row r="362">
-      <c r="A362" s="3"/>
-      <c r="B362" s="4" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C362" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D362" s="5" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E362" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F362" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G362" s="3"/>
-    </row>
-    <row r="363">
-      <c r="A363" s="3"/>
-      <c r="B363" s="4" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C363" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D363" s="5" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E363" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F363" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G363" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -54523,26 +54485,26 @@
     <hyperlink r:id="rId713" ref="E240"/>
     <hyperlink r:id="rId714" ref="F240"/>
     <hyperlink r:id="rId715" ref="D241"/>
-    <hyperlink r:id="rId716" ref="E241"/>
-    <hyperlink r:id="rId717" ref="F241"/>
-    <hyperlink r:id="rId718" ref="D242"/>
-    <hyperlink r:id="rId719" ref="E242"/>
-    <hyperlink r:id="rId720" ref="F242"/>
-    <hyperlink r:id="rId721" ref="D243"/>
+    <hyperlink r:id="rId716" ref="F241"/>
+    <hyperlink r:id="rId717" ref="D242"/>
+    <hyperlink r:id="rId718" ref="E242"/>
+    <hyperlink r:id="rId719" ref="F242"/>
+    <hyperlink r:id="rId720" ref="D243"/>
+    <hyperlink r:id="rId721" ref="E243"/>
     <hyperlink r:id="rId722" ref="F243"/>
     <hyperlink r:id="rId723" ref="D244"/>
     <hyperlink r:id="rId724" ref="E244"/>
-    <hyperlink r:id="rId725" ref="F244"/>
-    <hyperlink r:id="rId726" ref="D245"/>
-    <hyperlink r:id="rId727" ref="E245"/>
-    <hyperlink r:id="rId728" ref="F245"/>
-    <hyperlink r:id="rId729" ref="D246"/>
-    <hyperlink r:id="rId730" ref="E246"/>
-    <hyperlink r:id="rId731" ref="D247"/>
-    <hyperlink r:id="rId732" ref="E247"/>
-    <hyperlink r:id="rId733" ref="F247"/>
-    <hyperlink r:id="rId734" ref="D248"/>
-    <hyperlink r:id="rId735" ref="E248"/>
+    <hyperlink r:id="rId725" ref="D245"/>
+    <hyperlink r:id="rId726" ref="E245"/>
+    <hyperlink r:id="rId727" ref="F245"/>
+    <hyperlink r:id="rId728" ref="D246"/>
+    <hyperlink r:id="rId729" ref="E246"/>
+    <hyperlink r:id="rId730" ref="D247"/>
+    <hyperlink r:id="rId731" ref="E247"/>
+    <hyperlink r:id="rId732" ref="F247"/>
+    <hyperlink r:id="rId733" ref="D248"/>
+    <hyperlink r:id="rId734" ref="E248"/>
+    <hyperlink r:id="rId735" ref="F248"/>
     <hyperlink r:id="rId736" ref="D249"/>
     <hyperlink r:id="rId737" ref="E249"/>
     <hyperlink r:id="rId738" ref="F249"/>
@@ -54877,17 +54839,11 @@
     <hyperlink r:id="rId1067" ref="E359"/>
     <hyperlink r:id="rId1068" ref="F359"/>
     <hyperlink r:id="rId1069" ref="D360"/>
-    <hyperlink r:id="rId1070" ref="E360"/>
-    <hyperlink r:id="rId1071" ref="F360"/>
-    <hyperlink r:id="rId1072" ref="D361"/>
-    <hyperlink r:id="rId1073" ref="E361"/>
-    <hyperlink r:id="rId1074" ref="F361"/>
-    <hyperlink r:id="rId1075" ref="D362"/>
-    <hyperlink r:id="rId1076" ref="F362"/>
-    <hyperlink r:id="rId1077" ref="D363"/>
-    <hyperlink r:id="rId1078" ref="F363"/>
+    <hyperlink r:id="rId1070" ref="F360"/>
+    <hyperlink r:id="rId1071" ref="D361"/>
+    <hyperlink r:id="rId1072" ref="F361"/>
   </hyperlinks>
-  <drawing r:id="rId1079"/>
+  <drawing r:id="rId1073"/>
 </worksheet>
 </file>
 

</xml_diff>